<commit_message>
Refresh.  Adjusted Close Rate correction
</commit_message>
<xml_diff>
--- a/Session/Annual.xlsx
+++ b/Session/Annual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdang\source\repos\DDRINQ\Session\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400CA0F4-9F19-4BCC-85C8-E1764A3C3A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5082694-2C99-47F2-8308-76E31C1FEB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{8CA18F37-2DAB-41C4-ADD2-73D1823D0F11}"/>
   </bookViews>
@@ -295,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -362,9 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5490,7 +5487,7 @@
   <dimension ref="C2:K42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -6303,7 +6300,7 @@
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.45">
-      <c r="C38" s="31">
+      <c r="C38" s="29">
         <v>45338</v>
       </c>
       <c r="D38" s="5">

</xml_diff>